<commit_message>
Add values to config file and moved input excel to input folder
</commit_message>
<xml_diff>
--- a/REFramework_BlaackBook/Data/Config.xlsx
+++ b/REFramework_BlaackBook/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/mshanmug_stevens_edu/Documents/Documents/GitHub/Automation-Projects/REFramework_BlaackBook/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AC886EF9-44D0-4BB2-8F52-076E73C51AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9095C9EB-4544-408E-BCF0-D622BDB7E9EF}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{AC886EF9-44D0-4BB2-8F52-076E73C51AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{605E1F6D-0039-4C4C-88AA-4D5038C06F77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,9 +174,6 @@
     <t>https://api.nal.usda.gov/fdc/v1/foods/search?query=(FruitName)api_key=W1RMEcVF8BZAOLcOJcTJ7ZxzsoUNbEsKr8BJg67n</t>
   </si>
   <si>
-    <t>Blackbook.xlsx</t>
-  </si>
-  <si>
     <t>FoodWebsiteURL</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>https://www.taste.com.au</t>
+  </si>
+  <si>
+    <t>data/input/Blackbook.xlsx</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -669,10 +669,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -680,7 +680,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -693,18 +693,18 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
         <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Chnage of API end point in config file
</commit_message>
<xml_diff>
--- a/REFramework_BlaackBook/Data/Config.xlsx
+++ b/REFramework_BlaackBook/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/mshanmug_stevens_edu/Documents/Documents/GitHub/Automation-Projects/REFramework_BlaackBook/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{AC886EF9-44D0-4BB2-8F52-076E73C51AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{605E1F6D-0039-4C4C-88AA-4D5038C06F77}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AC886EF9-44D0-4BB2-8F52-076E73C51AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97B30072-051F-4527-BCEA-4547DEA7B123}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>APIEndPoint</t>
   </si>
   <si>
-    <t>https://api.nal.usda.gov/fdc/v1/foods/search?query=(FruitName)api_key=W1RMEcVF8BZAOLcOJcTJ7ZxzsoUNbEsKr8BJg67n</t>
-  </si>
-  <si>
     <t>FoodWebsiteURL</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>data/input/Blackbook.xlsx</t>
+  </si>
+  <si>
+    <t>https://api.nal.usda.gov/fdc/v1/foods/search?query={FruitName}api_key=W1RMEcVF8BZAOLcOJcTJ7ZxzsoUNbEsKr8BJg67n</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -669,10 +669,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -680,7 +680,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -688,23 +688,23 @@
         <v>47</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Final chnages. Added retry for get receipe sequence
</commit_message>
<xml_diff>
--- a/REFramework_BlaackBook/Data/Config.xlsx
+++ b/REFramework_BlaackBook/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/mshanmug_stevens_edu/Documents/Documents/GitHub/Automation-Projects/REFramework_BlaackBook/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AC886EF9-44D0-4BB2-8F52-076E73C51AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97B30072-051F-4527-BCEA-4547DEA7B123}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{AC886EF9-44D0-4BB2-8F52-076E73C51AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91A0C926-CBF1-4D32-9430-E8A769BCD558}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,7 +192,7 @@
     <t>data/input/Blackbook.xlsx</t>
   </si>
   <si>
-    <t>https://api.nal.usda.gov/fdc/v1/foods/search?query={FruitName}api_key=W1RMEcVF8BZAOLcOJcTJ7ZxzsoUNbEsKr8BJg67n</t>
+    <t>https://api.nal.usda.gov/fdc/v1/foods/search?query={FruitName}&amp;pageSize=2&amp;api_key=W1RMEcVF8BZAOLcOJcTJ7ZxzsoUNbEsKr8BJg67n</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1710,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1863,7 +1863,7 @@
         <v>34</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -1874,7 +1874,7 @@
         <v>35</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>

</xml_diff>